<commit_message>
Adicionando mensagens e eventos na tabela
</commit_message>
<xml_diff>
--- a/arquivos/ComprasOnline.xlsx
+++ b/arquivos/ComprasOnline.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -79,7 +79,13 @@
     <t>codigo_produto</t>
   </si>
   <si>
-    <t>local_produto</t>
+    <t>codigo_mensagem</t>
+  </si>
+  <si>
+    <t>mensagem</t>
+  </si>
+  <si>
+    <t>evento</t>
   </si>
   <si>
     <t>usuario_nome</t>
@@ -124,7 +130,7 @@
     <t>Silva</t>
   </si>
   <si>
-    <t>lista</t>
+    <t>adicionar-lista</t>
   </si>
   <si>
     <t>joaosilva</t>
@@ -196,7 +202,7 @@
     <t>Oliveira</t>
   </si>
   <si>
-    <t>estoque</t>
+    <t>adicionar-estoque</t>
   </si>
   <si>
     <t>Zezé_99</t>
@@ -247,9 +253,6 @@
     <t>fsociety12</t>
   </si>
   <si>
-    <t>Café</t>
-  </si>
-  <si>
     <t>RJ</t>
   </si>
   <si>
@@ -259,12 +262,6 @@
     <t>Leblon</t>
   </si>
   <si>
-    <t>Mundial</t>
-  </si>
-  <si>
-    <t>Três Corações</t>
-  </si>
-  <si>
     <t>29169-004</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
     <t>Alderson</t>
   </si>
   <si>
+    <t>adicionar-administrador</t>
+  </si>
+  <si>
     <t>elliotfs</t>
   </si>
   <si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>20matarxd</t>
+  </si>
+  <si>
+    <t>[...]Texto[...]</t>
+  </si>
+  <si>
+    <t>adicionar-mensagem</t>
   </si>
 </sst>
 </file>
@@ -521,7 +527,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="AF1:AF10" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="AF1:AF11" displayName="Table_1" id="1">
   <tableColumns count="1">
     <tableColumn name="usuario_nome" id="1"/>
   </tableColumns>
@@ -558,8 +564,10 @@
     <col customWidth="1" min="19" max="19" width="19.86"/>
     <col customWidth="1" min="20" max="20" width="22.86"/>
     <col customWidth="1" min="21" max="21" width="21.57"/>
-    <col customWidth="1" min="22" max="24" width="14.43"/>
-    <col customWidth="1" min="25" max="25" width="17.14"/>
+    <col customWidth="1" min="22" max="22" width="15.43"/>
+    <col customWidth="1" min="23" max="23" width="17.29"/>
+    <col customWidth="1" min="24" max="24" width="14.43"/>
+    <col customWidth="1" min="25" max="25" width="23.71"/>
     <col customWidth="1" min="26" max="26" width="14.43"/>
     <col customWidth="1" min="27" max="27" width="13.14"/>
     <col customWidth="1" min="28" max="32" width="14.43"/>
@@ -635,8 +643,12 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
@@ -644,7 +656,7 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -652,16 +664,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="7">
         <v>35197.0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F2" s="6">
         <v>5.0</v>
@@ -669,56 +681,62 @@
       <c r="G2" s="6">
         <v>5.0</v>
       </c>
-      <c r="H2" s="7">
-        <v>43545.0</v>
+      <c r="H2" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J2" s="6">
         <v>13.0</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P2" s="8">
         <v>5.0</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V2" s="9">
         <v>1.111111111E9</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="AF2" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -726,16 +744,16 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="7">
         <v>33056.0</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="6">
         <v>0.0</v>
@@ -743,56 +761,62 @@
       <c r="G3" s="6">
         <v>2.0</v>
       </c>
-      <c r="H3" s="7">
-        <v>43575.0</v>
+      <c r="H3" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="6">
         <v>10.0</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P3" s="8">
         <v>2.0</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="S3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="V3" s="9">
         <v>2.222222222E9</v>
       </c>
       <c r="W3" s="9" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -800,16 +824,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" s="7">
         <v>36412.0</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" s="6">
         <v>2.0</v>
@@ -821,52 +845,58 @@
         <v>43516.0</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J4" s="6">
         <v>15.0</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="P4" s="8">
         <v>3.0</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="V4" s="9">
         <v>3.333333333E9</v>
       </c>
       <c r="W4" s="9" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="AF4" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -874,16 +904,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C5" s="12">
         <v>36883.0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F5" s="6">
         <v>2.0</v>
@@ -891,56 +921,62 @@
       <c r="G5" s="6">
         <v>4.0</v>
       </c>
-      <c r="H5" s="7">
-        <v>43535.0</v>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J5" s="6">
         <v>5.0</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P5" s="8">
         <v>500.0</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="V5" s="9">
         <v>4.444444444E9</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -948,70 +984,76 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="7">
         <v>29718.0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>43477.0</v>
+        <v>79</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J6" s="6">
         <v>30.0</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="N6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="N6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="P6" s="8">
-        <v>250.0</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="S6" s="5" t="b">
         <v>1</v>
       </c>
       <c r="T6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="U6" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="V6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="V6" s="9">
-        <v>5.555555555E9</v>
-      </c>
-      <c r="W6" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="AF6" s="10" t="s">
         <v>87</v>
@@ -1022,16 +1064,16 @@
         <v>4.0</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C7" s="12">
         <v>36883.0</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" s="6">
         <v>2.0</v>
@@ -1049,16 +1091,16 @@
         <v>5.0</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>89</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>90</v>
@@ -1067,7 +1109,7 @@
         <v>270.0</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>91</v>
@@ -1076,19 +1118,25 @@
         <v>0</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="V7" s="9">
         <v>6.666666666E9</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -1096,16 +1144,16 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7">
         <v>35197.0</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" s="6">
         <v>5.0</v>
@@ -1123,16 +1171,16 @@
         <v>13.0</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>93</v>
@@ -1141,7 +1189,7 @@
         <v>1.0</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>94</v>
@@ -1150,19 +1198,25 @@
         <v>0</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V8" s="9">
         <v>7.777777777E9</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="AF8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -1170,16 +1224,16 @@
         <v>2.0</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="7">
         <v>33056.0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9" s="6">
         <v>1.0</v>
@@ -1191,31 +1245,31 @@
         <v>43575.0</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J9" s="6">
         <v>10.0</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P9" s="8">
         <v>2.0</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>95</v>
@@ -1224,19 +1278,25 @@
         <v>0</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="V9" s="9">
         <v>8.888888888E9</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>61</v>
+        <v>29</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y9" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -1261,17 +1321,17 @@
       <c r="G10" s="6">
         <v>5.0</v>
       </c>
-      <c r="H10" s="7">
-        <v>43606.0</v>
+      <c r="H10" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J10" s="6">
         <v>5.0</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>99</v>
@@ -1280,7 +1340,7 @@
         <v>100</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O10" s="6" t="s">
         <v>101</v>
@@ -1289,7 +1349,7 @@
         <v>2.0</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>102</v>
@@ -1307,16 +1367,95 @@
         <v>9.999999999E9</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="X10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y10" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="AF10" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="T11" s="13"/>
-      <c r="AA11" s="14"/>
-      <c r="AF11" s="15"/>
+    <row r="11" ht="17.25" customHeight="1">
+      <c r="A11" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="7">
+        <v>35197.0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="W11" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="X11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF11" s="10"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="T12" s="13"/>

</xml_diff>